<commit_message>
updated make metadata range
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_metadata.xlsx
+++ b/data-raw/metadata/feather_metadata.xlsx
@@ -6,13 +6,187 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="coverage" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="dataset" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="personnel" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="title" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="keyword_set" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="license" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="project" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="funding" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="maintenance" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="coverage" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="taxonomic_coverage" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geometry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monitoring juvenile Chinook salmon outmigration using rotary screw traps on the Feather River</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tabular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">last_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orcid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kindopp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jason.kindopp@water.ca.gov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">creator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">California Department of Water Resources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kassie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hickey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kassie.hickey@water.ca.gov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">principal investigator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ryon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kurth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ryon.kurth@water.ca.gov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">associate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">short_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monitoring juvenile Chinook salmon outmigration using rotary screw traps on Feather River</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feather River RST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keyword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keywordThesaurus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spring run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fall run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">catch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">juvenile production estimate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oncorhynchus tshawytscha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">California</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Valley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default_license</t>
+  </si>
+  <si>
+    <t xml:space="preserve">license_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">license_url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">license_identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intellectual_rights_description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">funder_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">funder_identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">award_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">award_title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">award_url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">funding_description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">update_frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ongoing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monthly</t>
+  </si>
   <si>
     <t xml:space="preserve">geographic_description</t>
   </si>
@@ -36,6 +210,39 @@
   </si>
   <si>
     <t xml:space="preserve">Feather River Rotary Screw Trap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CVPIA_common_species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">common_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phylum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taxon_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chinook</t>
   </si>
 </sst>
 </file>
@@ -385,22 +592,466 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>62</v>
       </c>
       <c r="B2" t="n">
         <v>-121.632636</v>

</xml_diff>

<commit_message>
testing for upload zip metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_metadata.xlsx
+++ b/data-raw/metadata/feather_metadata.xlsx
@@ -250,7 +250,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd hh:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="yyyy/mm/dd hh:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -288,7 +288,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1069,7 +1069,7 @@
         <v>35786</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>45408</v>
+        <v>45468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated link and files
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_metadata.xlsx
+++ b/data-raw/metadata/feather_metadata.xlsx
@@ -250,7 +250,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd hh:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="yyyy/mm/dd hh:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -288,7 +288,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1069,7 +1069,7 @@
         <v>35786</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>45408</v>
+        <v>45468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>